<commit_message>
Actualizo datos de las asignaturas2
</commit_message>
<xml_diff>
--- a/otros/HORARIOS.xlsx
+++ b/otros/HORARIOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/990a4fc8e327d43a/Documents/SEGUNDO/otros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C0ED15A-5FC3-4E4A-8706-AF911A07E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="8_{6C0ED15A-5FC3-4E4A-8706-AF911A07E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07E6AF93-FD83-4054-B7CA-45F1BD9A966A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{E23033B2-31BA-48FE-AC45-FBD6738E72D9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>Lunes</t>
   </si>
@@ -78,6 +78,45 @@
   </si>
   <si>
     <t>ING</t>
+  </si>
+  <si>
+    <t>Programacion multimedia y dispositivos moviles</t>
+  </si>
+  <si>
+    <t>Empresa e iniciativa emprendedora</t>
+  </si>
+  <si>
+    <t>Ingles</t>
+  </si>
+  <si>
+    <t>Acceso a datos</t>
+  </si>
+  <si>
+    <t>Sistemas de gestion empresarial</t>
+  </si>
+  <si>
+    <t>Programacion de servicios y procesos</t>
+  </si>
+  <si>
+    <t>Desarrollo de interfaces</t>
+  </si>
+  <si>
+    <t>Viernes</t>
+  </si>
+  <si>
+    <t>TRABAJOTE</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>LI</t>
   </si>
 </sst>
 </file>
@@ -106,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,73 +194,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -239,184 +224,59 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF698FB-96B0-441C-B14E-AFDA6B188BF9}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,135 +604,254 @@
     <col min="3" max="3" width="17.81640625" customWidth="1"/>
     <col min="4" max="4" width="17.90625" customWidth="1"/>
     <col min="5" max="5" width="18.08984375" customWidth="1"/>
+    <col min="6" max="6" width="23.453125" customWidth="1"/>
+    <col min="8" max="8" width="42.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4">
+      <c r="F2" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4">
+      <c r="F3" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="17">
         <v>0.37152777777777773</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" spans="1:5" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4">
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="17">
         <v>0.40625</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="30.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4">
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:8" ht="30.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="17">
         <v>0.4201388888888889</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="29.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4">
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" ht="29.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4">
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:8" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="17">
         <v>0.49652777777777773</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="11">
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="1:8" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="17">
         <v>0.51041666666666663</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="17">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="77.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="17">
+        <v>0.625</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G21" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="F3:F9"/>
+    <mergeCell ref="G21:H21"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>

</xml_diff>

<commit_message>
Actualizo datos de las asignaturas4
</commit_message>
<xml_diff>
--- a/otros/HORARIOS.xlsx
+++ b/otros/HORARIOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/990a4fc8e327d43a/Documents/SEGUNDO/otros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{6C0ED15A-5FC3-4E4A-8706-AF911A07E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07E6AF93-FD83-4054-B7CA-45F1BD9A966A}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="8_{6C0ED15A-5FC3-4E4A-8706-AF911A07E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90BD94FB-3610-4300-B514-C623BD539FE7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{E23033B2-31BA-48FE-AC45-FBD6738E72D9}"/>
   </bookViews>
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -246,18 +246,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -266,9 +255,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -277,6 +263,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,16 +593,12 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" customWidth="1"/>
-    <col min="6" max="6" width="23.453125" customWidth="1"/>
+    <col min="2" max="6" width="17" customWidth="1"/>
     <col min="8" max="8" width="42.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -623,42 +617,42 @@
       <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="36.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="17">
+    <row r="4" spans="1:8" ht="36.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="12">
         <v>0.37152777777777773</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="21"/>
-    </row>
-    <row r="5" spans="1:8" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="17">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="12">
         <v>0.40625</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -673,10 +667,10 @@
       <c r="E5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="21"/>
-    </row>
-    <row r="6" spans="1:8" ht="30.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="17">
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:8" ht="36.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="12">
         <v>0.4201388888888889</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -685,16 +679,16 @@
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:8" ht="29.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="17">
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" ht="36.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="12">
         <v>0.45833333333333331</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -703,14 +697,14 @@
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:8" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="17">
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="12">
         <v>0.49652777777777773</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -725,28 +719,28 @@
       <c r="E8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:8" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="17">
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" ht="36.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="12">
         <v>0.51041666666666663</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="17">
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="12">
         <v>0.54861111111111105</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -766,22 +760,22 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="77.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="17">
+      <c r="A11" s="12">
         <v>0.625</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -843,10 +837,10 @@
       </c>
     </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Actualizo datos de las asignaturas7
</commit_message>
<xml_diff>
--- a/otros/HORARIOS.xlsx
+++ b/otros/HORARIOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/990a4fc8e327d43a/Documents/SEGUNDO/otros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{6C0ED15A-5FC3-4E4A-8706-AF911A07E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90BD94FB-3610-4300-B514-C623BD539FE7}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{6C0ED15A-5FC3-4E4A-8706-AF911A07E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{618A58F7-B230-4ED4-B519-6E8902B12C8E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{E23033B2-31BA-48FE-AC45-FBD6738E72D9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>Lunes</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>LI</t>
+  </si>
+  <si>
+    <t>º</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -726,7 +729,7 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Actualizo datos de las asignaturas8
</commit_message>
<xml_diff>
--- a/otros/HORARIOS.xlsx
+++ b/otros/HORARIOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/990a4fc8e327d43a/Documents/SEGUNDO/otros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{6C0ED15A-5FC3-4E4A-8706-AF911A07E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{618A58F7-B230-4ED4-B519-6E8902B12C8E}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{6C0ED15A-5FC3-4E4A-8706-AF911A07E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9B00799-F32E-47D6-8775-55ABD4BC5F01}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{E23033B2-31BA-48FE-AC45-FBD6738E72D9}"/>
   </bookViews>
@@ -231,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,6 +259,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -294,6 +297,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -595,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF698FB-96B0-441C-B14E-AFDA6B188BF9}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -628,19 +635,19 @@
       <c r="A3" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -648,11 +655,11 @@
       <c r="A4" s="12">
         <v>0.37152777777777773</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="15"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12">
@@ -670,7 +677,7 @@
       <c r="E5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="36.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="12">
@@ -682,13 +689,13 @@
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="21" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="36.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="12">
@@ -700,11 +707,11 @@
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="15"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:8" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="12">
@@ -722,7 +729,7 @@
       <c r="E8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="36.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="12">
@@ -740,7 +747,7 @@
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:8" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="12">
@@ -840,10 +847,10 @@
       </c>
     </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="16"/>
+      <c r="H21" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>